<commit_message>
Add more tests to  unique titles in description and composition data
</commit_message>
<xml_diff>
--- a/input_data/data_errors_14/descricao.xlsx
+++ b/input_data/data_errors_14/descricao.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -136,12 +136,6 @@
     <t xml:space="preserve">4.2,6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacidade adaptativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Índice de capacidade adaptativa</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capacidade do sistema socioecológico de se ajustar a possíveis ameaças climáticas de seca.</t>
   </si>
   <si>
@@ -180,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -211,14 +205,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +217,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
         <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -314,11 +308,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,7 +508,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,7 +636,7 @@
       <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
@@ -676,7 +670,7 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>3</v>
       </c>
@@ -686,10 +680,10 @@
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="5" t="s">
         <v>23</v>
       </c>
@@ -723,20 +717,20 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
@@ -770,20 +764,20 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="5" t="s">
         <v>30</v>
       </c>
@@ -817,7 +811,7 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <v>6</v>
       </c>
@@ -830,7 +824,7 @@
       <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="5" t="s">
         <v>35</v>
       </c>
@@ -864,7 +858,7 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>7</v>
       </c>
@@ -872,17 +866,17 @@
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>0</v>
@@ -918,18 +912,18 @@
       <c r="B9" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
@@ -965,18 +959,18 @@
       <c r="B10" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
@@ -1008,14 +1002,14 @@
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1035,14 +1029,14 @@
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="5"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1062,14 +1056,14 @@
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
+      <c r="J13" s="9"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1089,14 +1083,14 @@
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1116,14 +1110,14 @@
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1143,14 +1137,14 @@
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1170,14 +1164,14 @@
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1197,14 +1191,14 @@
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -1224,14 +1218,14 @@
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="8"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -1251,14 +1245,14 @@
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -1278,14 +1272,14 @@
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
+      <c r="J21" s="9"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>

</xml_diff>